<commit_message>
Added readmes for each project
</commit_message>
<xml_diff>
--- a/Project/wecc_2020_unit_commitment/Input_descrptions_WECC_UC.xlsx
+++ b/Project/wecc_2020_unit_commitment/Input_descrptions_WECC_UC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdj2/Dropbox (Princeton)/Princeton/02 - Energy Systems Modeling Course/Test systems/wecc_2020_unit_commitment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdj2/power-systems-optimization/Project/wecc_2020_unit_commitment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187AD926-97DD-A347-8BD1-A869A4B96A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290132E4-B877-5845-ABDD-1CECCD8F70D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37680" yWindow="-2660" windowWidth="34680" windowHeight="16380" xr2:uid="{E2F8FAF9-854F-D04B-BF15-2CC6D544468C}"/>
   </bookViews>
@@ -408,9 +408,6 @@
   </si>
   <si>
     <t xml:space="preserve">Existing geneators are clustered at varying levels of resolution (in the Large, Medium, and Small versions) based on heat rate and fixed O&amp;M cost. </t>
-  </si>
-  <si>
-    <t>Demand follows EIA Annual Energy Outlook 2020 projected growth rates for load through 2040 (note: there is no modification of load profiles due to EV or heat pump electrification)</t>
   </si>
   <si>
     <t>This data set provides inputs for a unit commitment and/or economic dispatch study considering the existing generation in the Western Interconnection (Western Electricity Coordinating Council or WECC)</t>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>12. CO = WECC_CO (Colorado)</t>
+  </si>
+  <si>
+    <t>Demand profiles are based on 2012 weather year and are increased to 2020 values based on EIA Annual Energy Outlook data.</t>
   </si>
 </sst>
 </file>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1323AE-CE73-1247-9B89-544E97C0236E}">
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -947,7 +947,7 @@
     </row>
     <row r="2" spans="1:1" ht="17">
       <c r="A2" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17">
@@ -957,12 +957,12 @@
     </row>
     <row r="4" spans="1:1" ht="68">
       <c r="A4" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="17">
       <c r="A5" s="5" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -977,7 +977,7 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -987,67 +987,67 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to project data/readme.
Updates to WECC 2020 project data read-me (only one temporal resolution is provided not several)

Fixed ERCOT 52 week sample weights (1 period of 8760 hours instead of 1 period of 168 hours, which was incorrect).
</commit_message>
<xml_diff>
--- a/Project/wecc_2020_unit_commitment/Input_descrptions_WECC_UC.xlsx
+++ b/Project/wecc_2020_unit_commitment/Input_descrptions_WECC_UC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdj2/power-systems-optimization/Project/wecc_2020_unit_commitment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdj2/Documents/GitHub/power-systems-optimization/Project/wecc_2020_unit_commitment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290132E4-B877-5845-ABDD-1CECCD8F70D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ACEC34-4B70-DF40-8AD7-C4E03D623615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37680" yWindow="-2660" windowWidth="34680" windowHeight="16380" xr2:uid="{E2F8FAF9-854F-D04B-BF15-2CC6D544468C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E2F8FAF9-854F-D04B-BF15-2CC6D544468C}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="7" r:id="rId1"/>
@@ -410,35 +410,6 @@
     <t xml:space="preserve">Existing geneators are clustered at varying levels of resolution (in the Large, Medium, and Small versions) based on heat rate and fixed O&amp;M cost. </t>
   </si>
   <si>
-    <t>This data set provides inputs for a unit commitment and/or economic dispatch study considering the existing generation in the Western Interconnection (Western Electricity Coordinating Council or WECC)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">There are 12 regions (see zonal ID map below) and time series data provided for several levels of temporal resolution (10 days, 4 weeks, 8 weeks, 16 weeks, and 52 weeks). Each representative period represents 1 or more other weeks throughout the time series. The number of hours represented by each 168 hour 7 day period is given by the Representative_Period_Weight input column in the Inputs_data.csv file. Representative weeks and weights are determined via K-means clustering to minimize error in wind, solar, hydropower and demand time series within each cluster as per Mallapragada et al. (2018), Impact of model resolution on scenario outcomes for electricity sector system expansion, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Energy </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">163 (DOI: https://doi.org/10.1016/j.energy.2018.08.015) and always include the peak demand week. </t>
-    </r>
-  </si>
-  <si>
     <t>Zones:</t>
   </si>
   <si>
@@ -482,13 +453,19 @@
   </si>
   <si>
     <t>Demand profiles are based on 2012 weather year and are increased to 2020 values based on EIA Annual Energy Outlook data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 12 regions (see zonal ID list and map in the [Input_descrptions_WECC_UC.xlsx](Input_descrptions_WECC_UC.xlsx) file) and time series data provided for an entire year. </t>
+  </si>
+  <si>
+    <t>This data set provides inputs for a unit commitment and/or economic dispatch study considering the existing generation in the Western Interconnection (Western Electricity Coordinating Council or WECC) circa 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,14 +482,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -931,123 +900,123 @@
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="186" style="4" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17">
+    <row r="1" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17">
+    <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="68">
+    <row r="4" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="17">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="4" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="4" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="4" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="4" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="4" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1064,7 +1033,7 @@
       <selection activeCell="Y2" sqref="Y2:Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -1097,7 +1066,7 @@
     <col min="33" max="33" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1105,7 +1074,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1206,7 +1175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="85">
+    <row r="3" spans="1:33" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1307,7 +1276,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1421,12 +1390,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1434,7 +1403,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1442,7 +1411,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1450,7 +1419,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1458,7 +1427,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1479,14 +1448,14 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1496,7 +1465,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1513,7 +1482,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="34">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1530,7 +1499,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1560,7 +1529,7 @@
       <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
@@ -1575,7 +1544,7 @@
     <col min="17" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1583,7 +1552,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34">
+    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1606,7 +1575,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="68">
+    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>104</v>
       </c>
@@ -1629,7 +1598,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
@@ -1665,7 +1634,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
@@ -1678,7 +1647,7 @@
     <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1686,7 +1655,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1715,7 +1684,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51">
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>104</v>
       </c>
@@ -1740,7 +1709,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>

</xml_diff>